<commit_message>
updated output files to reflect 11 holdouts
</commit_message>
<xml_diff>
--- a/output/groupings_dems_impeachment.xlsx
+++ b/output/groupings_dems_impeachment.xlsx
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +860,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP13"/>
+  <dimension ref="A1:AP12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2440,12 +2440,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rose</t>
+          <t>Torres Small</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Max</t>
+          <t>Xochitl</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -2455,19 +2455,19 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M11">
-        <v>53</v>
+        <v>50.9</v>
       </c>
       <c r="N11">
-        <v>46.6</v>
+        <v>49.1</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -2475,11 +2475,11 @@
         </is>
       </c>
       <c r="P11">
-        <v>6.4</v>
+        <v>1.8</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>more_than_5_points</t>
+          <t>5_points_or_less</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -2489,35 +2489,35 @@
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>NY-11</t>
+          <t>NM-02</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>lean republican</t>
+          <t>tossup</t>
         </is>
       </c>
       <c r="U11">
-        <v>729159</v>
+        <v>698524</v>
       </c>
       <c r="V11">
-        <v>66890</v>
+        <v>41600</v>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="X11">
-        <v>39.2</v>
+        <v>35.9</v>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="Z11">
-        <v>38.413</v>
+        <v>62.273</v>
       </c>
       <c r="AA11" t="inlineStr">
         <is>
@@ -2525,16 +2525,16 @@
         </is>
       </c>
       <c r="AB11">
-        <v>33.426</v>
+        <v>20.589</v>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -2543,16 +2543,16 @@
         </is>
       </c>
       <c r="AF11">
-        <v>43.5</v>
+        <v>39.9</v>
       </c>
       <c r="AG11">
-        <v>53.3</v>
+        <v>50.1</v>
       </c>
       <c r="AH11">
-        <v>51.6</v>
+        <v>44.9</v>
       </c>
       <c r="AI11">
-        <v>47.2</v>
+        <v>51.7</v>
       </c>
       <c r="AJ11" t="inlineStr">
         <is>
@@ -2561,26 +2561,26 @@
       </c>
       <c r="AK11" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AM11" t="inlineStr">
         <is>
-          <t>3611</t>
+          <t>3502</t>
         </is>
       </c>
       <c r="AN11" t="inlineStr">
         <is>
-          <t>H8NY11113</t>
+          <t>H8NM02248</t>
         </is>
       </c>
       <c r="AO11" t="inlineStr">
         <is>
-          <t>R000613</t>
+          <t>T000484</t>
         </is>
       </c>
       <c r="AP11">
-        <v>9.799999999999997</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="12">
@@ -2591,12 +2591,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Torres Small</t>
+          <t>Van Drew</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Xochitl</t>
+          <t>Jefferson</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2615,10 +2615,10 @@
         </is>
       </c>
       <c r="M12">
-        <v>50.9</v>
+        <v>52.9</v>
       </c>
       <c r="N12">
-        <v>49.1</v>
+        <v>45.2</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -2626,11 +2626,11 @@
         </is>
       </c>
       <c r="P12">
-        <v>1.8</v>
+        <v>7.7</v>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>5_points_or_less</t>
+          <t>more_than_5_points</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -2640,43 +2640,43 @@
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>NM-02</t>
+          <t>NJ-02</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>tossup</t>
+          <t>likely democratic</t>
         </is>
       </c>
       <c r="U12">
-        <v>698524</v>
+        <v>729824</v>
       </c>
       <c r="V12">
-        <v>41600</v>
+        <v>59785</v>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="X12">
-        <v>35.9</v>
+        <v>41.4</v>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="Z12">
-        <v>62.273</v>
+        <v>33.95399999999999</v>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AB12">
-        <v>20.589</v>
+        <v>24.78</v>
       </c>
       <c r="AC12" t="inlineStr">
         <is>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="AD12" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AE12" t="inlineStr">
@@ -2694,16 +2694,16 @@
         </is>
       </c>
       <c r="AF12">
-        <v>39.9</v>
+        <v>46</v>
       </c>
       <c r="AG12">
-        <v>50.1</v>
+        <v>50.6</v>
       </c>
       <c r="AH12">
-        <v>44.9</v>
+        <v>53.7</v>
       </c>
       <c r="AI12">
-        <v>51.7</v>
+        <v>45.5</v>
       </c>
       <c r="AJ12" t="inlineStr">
         <is>
@@ -2712,176 +2712,25 @@
       </c>
       <c r="AK12" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AM12" t="inlineStr">
         <is>
-          <t>3502</t>
+          <t>3402</t>
         </is>
       </c>
       <c r="AN12" t="inlineStr">
         <is>
-          <t>H8NM02248</t>
+          <t>H8NJ02166</t>
         </is>
       </c>
       <c r="AO12" t="inlineStr">
         <is>
-          <t>T000484</t>
+          <t>V000133</t>
         </is>
       </c>
       <c r="AP12">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Van Drew</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Jefferson</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>NJ</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="M13">
-        <v>52.9</v>
-      </c>
-      <c r="N13">
-        <v>45.2</v>
-      </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="P13">
-        <v>7.7</v>
-      </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>more_than_5_points</t>
-        </is>
-      </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>NJ-02</t>
-        </is>
-      </c>
-      <c r="T13" t="inlineStr">
-        <is>
-          <t>likely democratic</t>
-        </is>
-      </c>
-      <c r="U13">
-        <v>729824</v>
-      </c>
-      <c r="V13">
-        <v>59785</v>
-      </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="X13">
-        <v>41.4</v>
-      </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="Z13">
-        <v>33.95399999999999</v>
-      </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AB13">
-        <v>24.78</v>
-      </c>
-      <c r="AC13" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AD13" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AE13" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AF13">
-        <v>46</v>
-      </c>
-      <c r="AG13">
-        <v>50.6</v>
-      </c>
-      <c r="AH13">
-        <v>53.7</v>
-      </c>
-      <c r="AI13">
-        <v>45.5</v>
-      </c>
-      <c r="AJ13" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="AK13" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AM13" t="inlineStr">
-        <is>
-          <t>3402</t>
-        </is>
-      </c>
-      <c r="AN13" t="inlineStr">
-        <is>
-          <t>H8NJ02166</t>
-        </is>
-      </c>
-      <c r="AO13" t="inlineStr">
-        <is>
-          <t>V000133</t>
-        </is>
-      </c>
-      <c r="AP13">
         <v>4.600000000000001</v>
       </c>
     </row>
@@ -2942,7 +2791,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -2972,7 +2821,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3017,7 +2866,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -3047,7 +2896,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5">
@@ -3107,7 +2956,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -3137,7 +2986,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5">
@@ -3212,7 +3061,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -3242,7 +3091,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6">
@@ -3312,7 +3161,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -3342,7 +3191,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4479,7 +4328,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4506,6 +4355,18 @@
         <is>
           <t>11</t>
         </is>
+      </c>
+      <c r="H8" s="2">
+        <v>43741</v>
+      </c>
+      <c r="J8" s="2">
+        <v>43741</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <v>2019</v>
       </c>
       <c r="M8">
         <v>53</v>

</xml_diff>

<commit_message>
updated output files to reflect 9 holdouts
</commit_message>
<xml_diff>
--- a/output/groupings_dems_impeachment.xlsx
+++ b/output/groupings_dems_impeachment.xlsx
@@ -416,7 +416,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +860,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP12"/>
+  <dimension ref="A1:AP10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1987,12 +1987,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>McAdams</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Collin</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>C.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2002,19 +2007,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="M8">
-        <v>50.1</v>
+        <v>52.1</v>
       </c>
       <c r="N8">
-        <v>49.9</v>
+        <v>47.9</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -2022,7 +2027,7 @@
         </is>
       </c>
       <c r="P8">
-        <v>0.2</v>
+        <v>4.2</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -2031,75 +2036,70 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>Y</t>
+          <t>N</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>UT-04</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr">
-        <is>
-          <t>tossup</t>
+          <t>MN-07</t>
         </is>
       </c>
       <c r="U8">
-        <v>757607</v>
+        <v>663338</v>
       </c>
       <c r="V8">
-        <v>65081</v>
+        <v>52930</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="X8">
+        <v>40.7</v>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
+        </is>
+      </c>
+      <c r="Z8">
+        <v>10.608</v>
+      </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="AB8">
+        <v>21.486</v>
+      </c>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="AD8" t="inlineStr">
+        <is>
+          <t>ABOVE</t>
+        </is>
+      </c>
+      <c r="AE8" t="inlineStr">
+        <is>
+          <t>BELOW</t>
+        </is>
+      </c>
+      <c r="AF8">
         <v>30.8</v>
       </c>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="Z8">
-        <v>24.46599999999999</v>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AB8">
-        <v>28.153</v>
-      </c>
-      <c r="AC8" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AD8" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="AF8">
-        <v>32.4</v>
-      </c>
       <c r="AG8">
-        <v>39.1</v>
+        <v>61.4</v>
       </c>
       <c r="AH8">
-        <v>30.4</v>
+        <v>44</v>
       </c>
       <c r="AI8">
-        <v>67.59999999999999</v>
+        <v>53.7</v>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
@@ -2113,21 +2113,21 @@
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>4904</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="AN8" t="inlineStr">
         <is>
-          <t>H8UT04053</t>
+          <t>H2MN07014</t>
         </is>
       </c>
       <c r="AO8" t="inlineStr">
         <is>
-          <t>M001209</t>
+          <t>P000258</t>
         </is>
       </c>
       <c r="AP8">
-        <v>6.700000000000003</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="9">
@@ -2138,12 +2138,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>McBath</t>
+          <t>Torres Small</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Lucy</t>
+          <t>Xochitl</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2153,19 +2153,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M9">
-        <v>50.5</v>
+        <v>50.9</v>
       </c>
       <c r="N9">
-        <v>49.5</v>
+        <v>49.1</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -2173,7 +2173,7 @@
         </is>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
@@ -2187,35 +2187,35 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>GA-06</t>
+          <t>NM-02</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>lean republican</t>
+          <t>tossup</t>
         </is>
       </c>
       <c r="U9">
-        <v>731334</v>
+        <v>698524</v>
       </c>
       <c r="V9">
-        <v>82390</v>
+        <v>41600</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="X9">
-        <v>37.7</v>
+        <v>35.9</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="Z9">
-        <v>39.012</v>
+        <v>62.273</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
@@ -2223,34 +2223,34 @@
         </is>
       </c>
       <c r="AB9">
-        <v>59.079</v>
+        <v>20.589</v>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AF9">
-        <v>46.8</v>
+        <v>39.9</v>
       </c>
       <c r="AG9">
-        <v>48.3</v>
+        <v>50.1</v>
       </c>
       <c r="AH9">
-        <v>37.4</v>
+        <v>44.9</v>
       </c>
       <c r="AI9">
-        <v>60.9</v>
+        <v>51.7</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
@@ -2264,21 +2264,21 @@
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>1306</t>
+          <t>3502</t>
         </is>
       </c>
       <c r="AN9" t="inlineStr">
         <is>
-          <t>H8GA06393</t>
+          <t>H8NM02248</t>
         </is>
       </c>
       <c r="AO9" t="inlineStr">
         <is>
-          <t>M001208</t>
+          <t>T000484</t>
         </is>
       </c>
       <c r="AP9">
-        <v>1.5</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="10">
@@ -2289,17 +2289,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Van Drew</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Collin</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>C.</t>
+          <t>Jefferson</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -2309,19 +2304,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M10">
-        <v>52.1</v>
+        <v>52.9</v>
       </c>
       <c r="N10">
-        <v>47.9</v>
+        <v>45.2</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -2329,36 +2324,41 @@
         </is>
       </c>
       <c r="P10">
-        <v>4.2</v>
+        <v>7.7</v>
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>5_points_or_less</t>
+          <t>more_than_5_points</t>
         </is>
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="S10" t="inlineStr">
         <is>
-          <t>MN-07</t>
+          <t>NJ-02</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>likely democratic</t>
         </is>
       </c>
       <c r="U10">
-        <v>663338</v>
+        <v>729824</v>
       </c>
       <c r="V10">
-        <v>52930</v>
+        <v>59785</v>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="X10">
-        <v>40.7</v>
+        <v>41.4</v>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="Z10">
-        <v>10.608</v>
+        <v>33.95399999999999</v>
       </c>
       <c r="AA10" t="inlineStr">
         <is>
@@ -2374,7 +2374,7 @@
         </is>
       </c>
       <c r="AB10">
-        <v>21.486</v>
+        <v>24.78</v>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
@@ -2383,7 +2383,7 @@
       </c>
       <c r="AD10" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AE10" t="inlineStr">
@@ -2392,16 +2392,16 @@
         </is>
       </c>
       <c r="AF10">
-        <v>30.8</v>
+        <v>46</v>
       </c>
       <c r="AG10">
-        <v>61.4</v>
+        <v>50.6</v>
       </c>
       <c r="AH10">
-        <v>44</v>
+        <v>53.7</v>
       </c>
       <c r="AI10">
-        <v>53.7</v>
+        <v>45.5</v>
       </c>
       <c r="AJ10" t="inlineStr">
         <is>
@@ -2410,327 +2410,25 @@
       </c>
       <c r="AK10" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AM10" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>3402</t>
         </is>
       </c>
       <c r="AN10" t="inlineStr">
         <is>
-          <t>H2MN07014</t>
+          <t>H8NJ02166</t>
         </is>
       </c>
       <c r="AO10" t="inlineStr">
         <is>
-          <t>P000258</t>
+          <t>V000133</t>
         </is>
       </c>
       <c r="AP10">
-        <v>30.6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Torres Small</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Xochitl</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>NM</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="M11">
-        <v>50.9</v>
-      </c>
-      <c r="N11">
-        <v>49.1</v>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="P11">
-        <v>1.8</v>
-      </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>5_points_or_less</t>
-        </is>
-      </c>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>NM-02</t>
-        </is>
-      </c>
-      <c r="T11" t="inlineStr">
-        <is>
-          <t>tossup</t>
-        </is>
-      </c>
-      <c r="U11">
-        <v>698524</v>
-      </c>
-      <c r="V11">
-        <v>41600</v>
-      </c>
-      <c r="W11" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="X11">
-        <v>35.9</v>
-      </c>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="Z11">
-        <v>62.273</v>
-      </c>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="AB11">
-        <v>20.589</v>
-      </c>
-      <c r="AC11" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AD11" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="AE11" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AF11">
-        <v>39.9</v>
-      </c>
-      <c r="AG11">
-        <v>50.1</v>
-      </c>
-      <c r="AH11">
-        <v>44.9</v>
-      </c>
-      <c r="AI11">
-        <v>51.7</v>
-      </c>
-      <c r="AJ11" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="AK11" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="AM11" t="inlineStr">
-        <is>
-          <t>3502</t>
-        </is>
-      </c>
-      <c r="AN11" t="inlineStr">
-        <is>
-          <t>H8NM02248</t>
-        </is>
-      </c>
-      <c r="AO11" t="inlineStr">
-        <is>
-          <t>T000484</t>
-        </is>
-      </c>
-      <c r="AP11">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Van Drew</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Jefferson</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>NJ</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="M12">
-        <v>52.9</v>
-      </c>
-      <c r="N12">
-        <v>45.2</v>
-      </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="P12">
-        <v>7.7</v>
-      </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>more_than_5_points</t>
-        </is>
-      </c>
-      <c r="R12" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="S12" t="inlineStr">
-        <is>
-          <t>NJ-02</t>
-        </is>
-      </c>
-      <c r="T12" t="inlineStr">
-        <is>
-          <t>likely democratic</t>
-        </is>
-      </c>
-      <c r="U12">
-        <v>729824</v>
-      </c>
-      <c r="V12">
-        <v>59785</v>
-      </c>
-      <c r="W12" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="X12">
-        <v>41.4</v>
-      </c>
-      <c r="Y12" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="Z12">
-        <v>33.95399999999999</v>
-      </c>
-      <c r="AA12" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AB12">
-        <v>24.78</v>
-      </c>
-      <c r="AC12" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AD12" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AE12" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AF12">
-        <v>46</v>
-      </c>
-      <c r="AG12">
-        <v>50.6</v>
-      </c>
-      <c r="AH12">
-        <v>53.7</v>
-      </c>
-      <c r="AI12">
-        <v>45.5</v>
-      </c>
-      <c r="AJ12" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="AK12" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AM12" t="inlineStr">
-        <is>
-          <t>3402</t>
-        </is>
-      </c>
-      <c r="AN12" t="inlineStr">
-        <is>
-          <t>H8NJ02166</t>
-        </is>
-      </c>
-      <c r="AO12" t="inlineStr">
-        <is>
-          <t>V000133</t>
-        </is>
-      </c>
-      <c r="AP12">
         <v>4.600000000000001</v>
       </c>
     </row>
@@ -2776,7 +2474,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -2806,7 +2504,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5">
@@ -2866,7 +2564,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -2881,7 +2579,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -2896,7 +2594,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5">
@@ -2911,7 +2609,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2956,7 +2654,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -2971,7 +2669,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -2986,7 +2684,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5">
@@ -3001,7 +2699,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3061,7 +2759,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -3091,7 +2789,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6">
@@ -3146,7 +2844,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -3176,7 +2874,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -4823,7 +4521,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4850,6 +4548,18 @@
         <is>
           <t>4</t>
         </is>
+      </c>
+      <c r="H11" s="2">
+        <v>43742</v>
+      </c>
+      <c r="J11" s="2">
+        <v>43742</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>2019</v>
       </c>
       <c r="M11">
         <v>50.1</v>
@@ -7279,7 +6989,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -7306,6 +7016,18 @@
         <is>
           <t>6</t>
         </is>
+      </c>
+      <c r="H26" s="2">
+        <v>43742</v>
+      </c>
+      <c r="J26" s="2">
+        <v>43742</v>
+      </c>
+      <c r="K26">
+        <v>10</v>
+      </c>
+      <c r="L26">
+        <v>2019</v>
       </c>
       <c r="M26">
         <v>50.5</v>

</xml_diff>

<commit_message>
updated output files to reflect 8 holdouts
</commit_message>
<xml_diff>
--- a/output/groupings_dems_impeachment.xlsx
+++ b/output/groupings_dems_impeachment.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -392,7 +392,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -401,28 +401,28 @@
         </is>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -431,21 +431,6 @@
         </is>
       </c>
       <c r="C4">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="C5">
         <v>23</v>
       </c>
     </row>
@@ -860,7 +845,7 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AP10"/>
+  <dimension ref="A1:AP9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1690,17 +1675,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Kind</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Eddie</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Bernice</t>
+          <t>Ron</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1710,19 +1690,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>WI</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>3</t>
         </is>
       </c>
       <c r="M6">
-        <v>91.09999999999999</v>
+        <v>59.7</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>40.3</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
@@ -1730,7 +1710,7 @@
         </is>
       </c>
       <c r="P6">
-        <v>91.09999999999999</v>
+        <v>19.4</v>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
@@ -1744,14 +1724,14 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>TX-30</t>
+          <t>WI-03</t>
         </is>
       </c>
       <c r="U6">
-        <v>745784</v>
+        <v>718576</v>
       </c>
       <c r="V6">
-        <v>42708</v>
+        <v>50985</v>
       </c>
       <c r="W6" t="inlineStr">
         <is>
@@ -1759,23 +1739,23 @@
         </is>
       </c>
       <c r="X6">
-        <v>32.8</v>
+        <v>38.4</v>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="Z6">
-        <v>84.529</v>
+        <v>7.597999999999999</v>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AB6">
-        <v>19.847</v>
+        <v>24.286</v>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
@@ -1784,29 +1764,29 @@
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AF6">
-        <v>79.09999999999999</v>
+        <v>44.3</v>
       </c>
       <c r="AG6">
-        <v>18.3</v>
+        <v>48.8</v>
       </c>
       <c r="AH6">
-        <v>79.59999999999999</v>
+        <v>54.7</v>
       </c>
       <c r="AI6">
-        <v>19.6</v>
+        <v>43.7</v>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
@@ -1816,21 +1796,21 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>4830</t>
+          <t>5503</t>
         </is>
       </c>
       <c r="AN6" t="inlineStr">
         <is>
-          <t>H2TX00015</t>
+          <t>H6WI03099</t>
         </is>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
-          <t>J000126</t>
+          <t>K000188</t>
         </is>
       </c>
       <c r="AP6">
-        <v>-60.8</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="7">
@@ -1841,12 +1821,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kind</t>
+          <t>Peterson</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ron</t>
+          <t>Collin</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>C.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1856,19 +1841,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>WI</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="M7">
-        <v>59.7</v>
+        <v>52.1</v>
       </c>
       <c r="N7">
-        <v>40.3</v>
+        <v>47.9</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
@@ -1876,11 +1861,11 @@
         </is>
       </c>
       <c r="P7">
-        <v>19.4</v>
+        <v>4.2</v>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>more_than_5_points</t>
+          <t>5_points_or_less</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
@@ -1890,14 +1875,14 @@
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>WI-03</t>
+          <t>MN-07</t>
         </is>
       </c>
       <c r="U7">
-        <v>718576</v>
+        <v>663338</v>
       </c>
       <c r="V7">
-        <v>50985</v>
+        <v>52930</v>
       </c>
       <c r="W7" t="inlineStr">
         <is>
@@ -1905,7 +1890,7 @@
         </is>
       </c>
       <c r="X7">
-        <v>38.4</v>
+        <v>40.7</v>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
@@ -1913,7 +1898,7 @@
         </is>
       </c>
       <c r="Z7">
-        <v>7.597999999999999</v>
+        <v>10.608</v>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
@@ -1921,7 +1906,7 @@
         </is>
       </c>
       <c r="AB7">
-        <v>24.286</v>
+        <v>21.486</v>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
@@ -1939,16 +1924,16 @@
         </is>
       </c>
       <c r="AF7">
-        <v>44.3</v>
+        <v>30.8</v>
       </c>
       <c r="AG7">
-        <v>48.8</v>
+        <v>61.4</v>
       </c>
       <c r="AH7">
-        <v>54.7</v>
+        <v>44</v>
       </c>
       <c r="AI7">
-        <v>43.7</v>
+        <v>53.7</v>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
@@ -1957,26 +1942,26 @@
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>R</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>5503</t>
+          <t>2707</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr">
         <is>
-          <t>H6WI03099</t>
+          <t>H2MN07014</t>
         </is>
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>K000188</t>
+          <t>P000258</t>
         </is>
       </c>
       <c r="AP7">
-        <v>4.5</v>
+        <v>30.6</v>
       </c>
     </row>
     <row r="8">
@@ -1987,17 +1972,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Peterson</t>
+          <t>Torres Small</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Collin</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>C.</t>
+          <t>Xochitl</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -2007,19 +1987,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M8">
-        <v>52.1</v>
+        <v>50.9</v>
       </c>
       <c r="N8">
-        <v>47.9</v>
+        <v>49.1</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -2027,7 +2007,7 @@
         </is>
       </c>
       <c r="P8">
-        <v>4.2</v>
+        <v>1.8</v>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
@@ -2036,19 +2016,24 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>N</t>
+          <t>Y</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>MN-07</t>
+          <t>NM-02</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>tossup</t>
         </is>
       </c>
       <c r="U8">
-        <v>663338</v>
+        <v>698524</v>
       </c>
       <c r="V8">
-        <v>52930</v>
+        <v>41600</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
@@ -2056,23 +2041,23 @@
         </is>
       </c>
       <c r="X8">
-        <v>40.7</v>
+        <v>35.9</v>
       </c>
       <c r="Y8" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="Z8">
-        <v>10.608</v>
+        <v>62.273</v>
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="AB8">
-        <v>21.486</v>
+        <v>20.589</v>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
@@ -2090,16 +2075,16 @@
         </is>
       </c>
       <c r="AF8">
-        <v>30.8</v>
+        <v>39.9</v>
       </c>
       <c r="AG8">
-        <v>61.4</v>
+        <v>50.1</v>
       </c>
       <c r="AH8">
-        <v>44</v>
+        <v>44.9</v>
       </c>
       <c r="AI8">
-        <v>53.7</v>
+        <v>51.7</v>
       </c>
       <c r="AJ8" t="inlineStr">
         <is>
@@ -2113,21 +2098,21 @@
       </c>
       <c r="AM8" t="inlineStr">
         <is>
-          <t>2707</t>
+          <t>3502</t>
         </is>
       </c>
       <c r="AN8" t="inlineStr">
         <is>
-          <t>H2MN07014</t>
+          <t>H8NM02248</t>
         </is>
       </c>
       <c r="AO8" t="inlineStr">
         <is>
-          <t>P000258</t>
+          <t>T000484</t>
         </is>
       </c>
       <c r="AP8">
-        <v>30.6</v>
+        <v>10.2</v>
       </c>
     </row>
     <row r="9">
@@ -2138,12 +2123,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Torres Small</t>
+          <t>Van Drew</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Xochitl</t>
+          <t>Jefferson</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -2153,7 +2138,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -2162,10 +2147,10 @@
         </is>
       </c>
       <c r="M9">
-        <v>50.9</v>
+        <v>52.9</v>
       </c>
       <c r="N9">
-        <v>49.1</v>
+        <v>45.2</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -2173,11 +2158,11 @@
         </is>
       </c>
       <c r="P9">
-        <v>1.8</v>
+        <v>7.7</v>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>5_points_or_less</t>
+          <t>more_than_5_points</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
@@ -2187,43 +2172,43 @@
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>NM-02</t>
+          <t>NJ-02</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>tossup</t>
+          <t>likely democratic</t>
         </is>
       </c>
       <c r="U9">
-        <v>698524</v>
+        <v>729824</v>
       </c>
       <c r="V9">
-        <v>41600</v>
+        <v>59785</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="X9">
-        <v>35.9</v>
+        <v>41.4</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>BELOW</t>
+          <t>ABOVE</t>
         </is>
       </c>
       <c r="Z9">
-        <v>62.273</v>
+        <v>33.95399999999999</v>
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AB9">
-        <v>20.589</v>
+        <v>24.78</v>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
@@ -2232,7 +2217,7 @@
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>ABOVE</t>
+          <t>BELOW</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
@@ -2241,16 +2226,16 @@
         </is>
       </c>
       <c r="AF9">
-        <v>39.9</v>
+        <v>46</v>
       </c>
       <c r="AG9">
-        <v>50.1</v>
+        <v>50.6</v>
       </c>
       <c r="AH9">
-        <v>44.9</v>
+        <v>53.7</v>
       </c>
       <c r="AI9">
-        <v>51.7</v>
+        <v>45.5</v>
       </c>
       <c r="AJ9" t="inlineStr">
         <is>
@@ -2259,176 +2244,25 @@
       </c>
       <c r="AK9" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>D</t>
         </is>
       </c>
       <c r="AM9" t="inlineStr">
         <is>
-          <t>3502</t>
+          <t>3402</t>
         </is>
       </c>
       <c r="AN9" t="inlineStr">
         <is>
-          <t>H8NM02248</t>
+          <t>H8NJ02166</t>
         </is>
       </c>
       <c r="AO9" t="inlineStr">
         <is>
-          <t>T000484</t>
+          <t>V000133</t>
         </is>
       </c>
       <c r="AP9">
-        <v>10.2</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Van Drew</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Jefferson</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>NJ</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="M10">
-        <v>52.9</v>
-      </c>
-      <c r="N10">
-        <v>45.2</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="P10">
-        <v>7.7</v>
-      </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>more_than_5_points</t>
-        </is>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>NJ-02</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>likely democratic</t>
-        </is>
-      </c>
-      <c r="U10">
-        <v>729824</v>
-      </c>
-      <c r="V10">
-        <v>59785</v>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="X10">
-        <v>41.4</v>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>ABOVE</t>
-        </is>
-      </c>
-      <c r="Z10">
-        <v>33.95399999999999</v>
-      </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AB10">
-        <v>24.78</v>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>BELOW</t>
-        </is>
-      </c>
-      <c r="AF10">
-        <v>46</v>
-      </c>
-      <c r="AG10">
-        <v>50.6</v>
-      </c>
-      <c r="AH10">
-        <v>53.7</v>
-      </c>
-      <c r="AI10">
-        <v>45.5</v>
-      </c>
-      <c r="AJ10" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-      <c r="AK10" t="inlineStr">
-        <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="AM10" t="inlineStr">
-        <is>
-          <t>3402</t>
-        </is>
-      </c>
-      <c r="AN10" t="inlineStr">
-        <is>
-          <t>H8NJ02166</t>
-        </is>
-      </c>
-      <c r="AO10" t="inlineStr">
-        <is>
-          <t>V000133</t>
-        </is>
-      </c>
-      <c r="AP10">
         <v>4.600000000000001</v>
       </c>
     </row>
@@ -2474,7 +2308,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -2504,7 +2338,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5">
@@ -2579,7 +2413,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -2609,7 +2443,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2654,7 +2488,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -2684,7 +2518,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5">
@@ -2759,7 +2593,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -2789,7 +2623,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6">
@@ -2859,7 +2693,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -2889,7 +2723,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>